<commit_message>
Corrección Anexión Datos Faltantes
</commit_message>
<xml_diff>
--- a/Datos/diccionario_propio.xlsx
+++ b/Datos/diccionario_propio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Desktop\Otros Proyectos\Encuesta Multiproposito\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E3BEC6-D4EE-49D5-9A3C-67E47DDA9F0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C649E1BA-C653-4E3E-A771-BA6C91A9274B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12103,10 +12103,10 @@
   <dimension ref="A1:H1596"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B208" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D207" sqref="D207"/>
+      <selection pane="bottomRight" activeCell="A211" sqref="A211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Casi se finaliza la sección NPFCP
</commit_message>
<xml_diff>
--- a/Datos/diccionario_propio.xlsx
+++ b/Datos/diccionario_propio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Desktop\Otros Proyectos\Encuesta Multiproposito\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0113C8-A7B0-4B08-A12C-848DB0812996}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ABE1E9-3D00-469E-9096-DDB10F1C3364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12103,10 +12103,10 @@
   <dimension ref="A1:J1596"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B362" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B400" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A416" sqref="A416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20599,23 +20599,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:7" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A373" s="39" t="s">
+    <row r="373" spans="1:7" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A373" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B373" s="24" t="s">
+      <c r="B373" s="47" t="s">
         <v>518</v>
       </c>
-      <c r="C373" s="27" t="s">
+      <c r="C373" s="46" t="s">
         <v>1869</v>
       </c>
-      <c r="D373" s="27" t="s">
+      <c r="D373" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E373" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F373" s="28">
+      <c r="E373" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F373" s="48">
         <v>8</v>
       </c>
       <c r="G373" s="29">
@@ -20784,22 +20784,22 @@
       </c>
     </row>
     <row r="381" spans="1:7" s="29" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A381" s="39" t="s">
+      <c r="A381" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B381" s="24" t="s">
+      <c r="B381" s="47" t="s">
         <v>526</v>
       </c>
-      <c r="C381" s="26" t="s">
+      <c r="C381" s="46" t="s">
         <v>2457</v>
       </c>
-      <c r="D381" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E381" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F381" s="28">
+      <c r="D381" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E381" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F381" s="48">
         <v>8</v>
       </c>
       <c r="G381" s="29">
@@ -20807,22 +20807,22 @@
       </c>
     </row>
     <row r="382" spans="1:7" s="29" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A382" s="39" t="s">
+      <c r="A382" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B382" s="24" t="s">
+      <c r="B382" s="47" t="s">
         <v>527</v>
       </c>
-      <c r="C382" s="26" t="s">
+      <c r="C382" s="46" t="s">
         <v>2458</v>
       </c>
-      <c r="D382" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E382" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F382" s="28">
+      <c r="D382" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E382" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F382" s="48">
         <v>8</v>
       </c>
       <c r="G382" s="29">
@@ -20830,22 +20830,22 @@
       </c>
     </row>
     <row r="383" spans="1:7" s="29" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A383" s="39" t="s">
+      <c r="A383" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B383" s="24" t="s">
+      <c r="B383" s="47" t="s">
         <v>528</v>
       </c>
-      <c r="C383" s="26" t="s">
+      <c r="C383" s="46" t="s">
         <v>2459</v>
       </c>
-      <c r="D383" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E383" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F383" s="28">
+      <c r="D383" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E383" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F383" s="48">
         <v>8</v>
       </c>
       <c r="G383" s="29">
@@ -20853,22 +20853,22 @@
       </c>
     </row>
     <row r="384" spans="1:7" s="29" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A384" s="39" t="s">
+      <c r="A384" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B384" s="24" t="s">
+      <c r="B384" s="47" t="s">
         <v>529</v>
       </c>
-      <c r="C384" s="26" t="s">
+      <c r="C384" s="46" t="s">
         <v>2460</v>
       </c>
-      <c r="D384" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E384" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F384" s="28">
+      <c r="D384" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E384" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F384" s="48">
         <v>8</v>
       </c>
       <c r="G384" s="29">
@@ -20876,22 +20876,22 @@
       </c>
     </row>
     <row r="385" spans="1:7" s="29" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A385" s="39" t="s">
+      <c r="A385" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B385" s="24" t="s">
+      <c r="B385" s="47" t="s">
         <v>530</v>
       </c>
-      <c r="C385" s="26" t="s">
+      <c r="C385" s="46" t="s">
         <v>2461</v>
       </c>
-      <c r="D385" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E385" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F385" s="28">
+      <c r="D385" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E385" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F385" s="48">
         <v>8</v>
       </c>
       <c r="G385" s="29">
@@ -20944,23 +20944,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:7" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A388" s="39" t="s">
+    <row r="388" spans="1:7" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A388" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B388" s="24" t="s">
+      <c r="B388" s="47" t="s">
         <v>533</v>
       </c>
-      <c r="C388" s="26" t="s">
+      <c r="C388" s="46" t="s">
         <v>1874</v>
       </c>
-      <c r="D388" s="27" t="s">
-        <v>3026</v>
-      </c>
-      <c r="E388" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F388" s="28">
+      <c r="D388" s="46" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E388" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F388" s="48">
         <v>8</v>
       </c>
       <c r="G388" s="29">
@@ -21566,22 +21566,22 @@
       </c>
     </row>
     <row r="415" spans="1:7" s="29" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A415" s="39" t="s">
+      <c r="A415" s="45" t="s">
         <v>489</v>
       </c>
-      <c r="B415" s="24" t="s">
+      <c r="B415" s="47" t="s">
         <v>548</v>
       </c>
-      <c r="C415" s="26" t="s">
+      <c r="C415" s="46" t="s">
         <v>1886</v>
       </c>
-      <c r="D415" s="26" t="s">
+      <c r="D415" s="46" t="s">
         <v>2473</v>
       </c>
-      <c r="E415" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F415" s="28">
+      <c r="E415" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F415" s="48">
         <v>8</v>
       </c>
       <c r="G415" s="29">

</xml_diff>

<commit_message>
Reorganizado todas las secciones de la encuesta
</commit_message>
<xml_diff>
--- a/Datos/diccionario_propio.xlsx
+++ b/Datos/diccionario_propio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Desktop\Otros Proyectos\Encuesta Multiproposito\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F9004F-C6F4-4D7E-913A-9CF398D8EAD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4537AD-7B89-448F-8AF9-F84AD979F624}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7564" uniqueCount="3184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37820" uniqueCount="3184">
   <si>
     <t>NOMBRE TABLA</t>
   </si>
@@ -11439,7 +11439,7 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -11655,9 +11655,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="4" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -11683,6 +11680,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12139,7 +12142,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B676" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A680" sqref="A680:F680"/>
+      <selection pane="bottomRight" activeCell="A768" sqref="A768:F768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18785,10 +18788,10 @@
         <v>1</v>
       </c>
       <c r="H291" s="32"/>
-      <c r="I291" s="73" t="s">
+      <c r="I291" s="82" t="s">
         <v>3183</v>
       </c>
-      <c r="J291" s="73"/>
+      <c r="J291" s="82"/>
     </row>
     <row r="292" spans="1:10" s="14" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="65" t="s">
@@ -18811,8 +18814,8 @@
         <v>1</v>
       </c>
       <c r="H292" s="32"/>
-      <c r="I292" s="73"/>
-      <c r="J292" s="73"/>
+      <c r="I292" s="82"/>
+      <c r="J292" s="82"/>
     </row>
     <row r="293" spans="1:10" s="14" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="43" t="s">
@@ -23856,22 +23859,22 @@
       </c>
     </row>
     <row r="514" spans="1:7" s="29" customFormat="1" ht="195" x14ac:dyDescent="0.2">
-      <c r="A514" s="74" t="s">
+      <c r="A514" s="73" t="s">
         <v>621</v>
       </c>
-      <c r="B514" s="75" t="s">
+      <c r="B514" s="74" t="s">
         <v>656</v>
       </c>
-      <c r="C514" s="76" t="s">
+      <c r="C514" s="75" t="s">
         <v>657</v>
       </c>
-      <c r="D514" s="76" t="s">
+      <c r="D514" s="75" t="s">
         <v>2536</v>
       </c>
-      <c r="E514" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="F514" s="77">
+      <c r="E514" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F514" s="76">
         <v>8</v>
       </c>
       <c r="G514" s="29">
@@ -27249,22 +27252,22 @@
       </c>
     </row>
     <row r="665" spans="1:7" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A665" s="78" t="s">
+      <c r="A665" s="77" t="s">
         <v>690</v>
       </c>
-      <c r="B665" s="79" t="s">
+      <c r="B665" s="78" t="s">
         <v>820</v>
       </c>
-      <c r="C665" s="80" t="s">
+      <c r="C665" s="79" t="s">
         <v>821</v>
       </c>
-      <c r="D665" s="81" t="s">
+      <c r="D665" s="80" t="s">
         <v>2636</v>
       </c>
-      <c r="E665" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="F665" s="82">
+      <c r="E665" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F665" s="81">
         <v>8</v>
       </c>
       <c r="G665" s="29">
@@ -27272,22 +27275,22 @@
       </c>
     </row>
     <row r="666" spans="1:7" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A666" s="78" t="s">
+      <c r="A666" s="77" t="s">
         <v>690</v>
       </c>
-      <c r="B666" s="79" t="s">
+      <c r="B666" s="78" t="s">
         <v>822</v>
       </c>
-      <c r="C666" s="81" t="s">
+      <c r="C666" s="80" t="s">
         <v>2535</v>
       </c>
-      <c r="D666" s="80" t="s">
+      <c r="D666" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="E666" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="F666" s="82">
+      <c r="E666" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F666" s="81">
         <v>8</v>
       </c>
       <c r="G666" s="29">
@@ -29592,20 +29595,20 @@
       </c>
     </row>
     <row r="768" spans="1:7" s="29" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A768" s="38" t="s">
+      <c r="A768" s="77" t="s">
         <v>925</v>
       </c>
-      <c r="B768" s="25" t="s">
+      <c r="B768" s="83" t="s">
         <v>939</v>
       </c>
-      <c r="C768" s="26" t="s">
+      <c r="C768" s="80" t="s">
         <v>2717</v>
       </c>
-      <c r="D768" s="26"/>
-      <c r="E768" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F768" s="28">
+      <c r="D768" s="80"/>
+      <c r="E768" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F768" s="81">
         <v>8</v>
       </c>
       <c r="G768" s="29">

</xml_diff>

<commit_message>
Inicio 9 Sección NCPKP
</commit_message>
<xml_diff>
--- a/Datos/diccionario_propio.xlsx
+++ b/Datos/diccionario_propio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Desktop\Otros Proyectos\Encuesta Multiproposito\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992B70E7-08D7-471D-8C45-841F051220E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D4AD9-3ECF-4F82-B49F-1D9960B3E09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11430,7 +11430,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -11438,6 +11438,9 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -11689,8 +11692,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Bueno" xfId="4" builtinId="26"/>
+    <cellStyle name="Estilo 1" xfId="7" xr:uid="{076A080A-000F-42CD-84D2-1B7C3F9144FD}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Incorrecto" xfId="5" builtinId="27"/>
     <cellStyle name="Neutral" xfId="6" builtinId="28"/>
@@ -12139,10 +12143,10 @@
   <dimension ref="A1:J1596"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B818" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B827" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C819" sqref="C819"/>
+      <selection pane="bottomRight" activeCell="A832" sqref="A832:F832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14494,7 +14498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" s="14" customFormat="1" ht="13.5" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A104" s="36" t="s">
         <v>119</v>
       </c>
@@ -14517,7 +14521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="14" customFormat="1" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" s="14" customFormat="1" ht="64.5" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A105" s="36" t="s">
         <v>119</v>
       </c>
@@ -14540,7 +14544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" s="14" customFormat="1" ht="13.5" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A106" s="36" t="s">
         <v>119</v>
       </c>
@@ -14563,7 +14567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" s="14" customFormat="1" ht="26.25" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A107" s="36" t="s">
         <v>119</v>
       </c>
@@ -14586,7 +14590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" s="14" customFormat="1" ht="39" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A108" s="36" t="s">
         <v>119</v>
       </c>
@@ -14609,7 +14613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="14" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" s="14" customFormat="1" ht="115.5" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A109" s="36" t="s">
         <v>119</v>
       </c>
@@ -27724,7 +27728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="686" spans="1:7" s="14" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:7" s="14" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A686" s="36" t="s">
         <v>840</v>
       </c>
@@ -27744,10 +27748,10 @@
         <v>1</v>
       </c>
       <c r="G686" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="687" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="687" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A687" s="36" t="s">
         <v>840</v>
       </c>
@@ -27767,10 +27771,10 @@
         <v>8</v>
       </c>
       <c r="G687" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="688" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="688" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A688" s="36" t="s">
         <v>840</v>
       </c>
@@ -27790,10 +27794,10 @@
         <v>8</v>
       </c>
       <c r="G688" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="689" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A689" s="36" t="s">
         <v>840</v>
       </c>
@@ -27813,10 +27817,10 @@
         <v>8</v>
       </c>
       <c r="G689" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="690" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="690" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A690" s="36" t="s">
         <v>840</v>
       </c>
@@ -27836,10 +27840,10 @@
         <v>8</v>
       </c>
       <c r="G690" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="691" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A691" s="36" t="s">
         <v>840</v>
       </c>
@@ -27859,10 +27863,10 @@
         <v>8</v>
       </c>
       <c r="G691" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="692" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A692" s="36" t="s">
         <v>840</v>
       </c>
@@ -27882,10 +27886,10 @@
         <v>8</v>
       </c>
       <c r="G692" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="693" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="693" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A693" s="36" t="s">
         <v>840</v>
       </c>
@@ -27905,10 +27909,10 @@
         <v>8</v>
       </c>
       <c r="G693" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="694" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="694" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A694" s="36" t="s">
         <v>840</v>
       </c>
@@ -27928,10 +27932,10 @@
         <v>8</v>
       </c>
       <c r="G694" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="695" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="695" spans="1:7" s="14" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A695" s="36" t="s">
         <v>840</v>
       </c>
@@ -27951,10 +27955,10 @@
         <v>8</v>
       </c>
       <c r="G695" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="696" spans="1:7" s="14" customFormat="1" ht="102" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="696" spans="1:7" s="14" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A696" s="36" t="s">
         <v>840</v>
       </c>
@@ -27974,10 +27978,10 @@
         <v>8</v>
       </c>
       <c r="G696" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="697" spans="1:7" s="14" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="697" spans="1:7" s="14" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A697" s="36" t="s">
         <v>840</v>
       </c>
@@ -27997,10 +28001,10 @@
         <v>8</v>
       </c>
       <c r="G697" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="698" spans="1:7" s="14" customFormat="1" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="698" spans="1:7" s="14" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A698" s="36" t="s">
         <v>840</v>
       </c>
@@ -28020,10 +28024,10 @@
         <v>8</v>
       </c>
       <c r="G698" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="699" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="699" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A699" s="36" t="s">
         <v>840</v>
       </c>
@@ -28043,10 +28047,10 @@
         <v>8</v>
       </c>
       <c r="G699" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="700" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="700" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A700" s="36" t="s">
         <v>840</v>
       </c>
@@ -28066,10 +28070,10 @@
         <v>8</v>
       </c>
       <c r="G700" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="701" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="701" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A701" s="36" t="s">
         <v>840</v>
       </c>
@@ -28089,10 +28093,10 @@
         <v>8</v>
       </c>
       <c r="G701" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="702" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="702" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A702" s="36" t="s">
         <v>840</v>
       </c>
@@ -28112,10 +28116,10 @@
         <v>8</v>
       </c>
       <c r="G702" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="703" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="703" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A703" s="36" t="s">
         <v>840</v>
       </c>
@@ -28135,10 +28139,10 @@
         <v>8</v>
       </c>
       <c r="G703" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="704" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A704" s="36" t="s">
         <v>840</v>
       </c>
@@ -28158,10 +28162,10 @@
         <v>8</v>
       </c>
       <c r="G704" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="705" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="705" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A705" s="36" t="s">
         <v>840</v>
       </c>
@@ -28181,10 +28185,10 @@
         <v>8</v>
       </c>
       <c r="G705" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="706" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A706" s="36" t="s">
         <v>840</v>
       </c>
@@ -28204,10 +28208,10 @@
         <v>8</v>
       </c>
       <c r="G706" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="707" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A707" s="36" t="s">
         <v>840</v>
       </c>
@@ -28227,10 +28231,10 @@
         <v>8</v>
       </c>
       <c r="G707" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="708" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A708" s="36" t="s">
         <v>840</v>
       </c>
@@ -28250,10 +28254,10 @@
         <v>8</v>
       </c>
       <c r="G708" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="709" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A709" s="36" t="s">
         <v>840</v>
       </c>
@@ -28273,10 +28277,10 @@
         <v>8</v>
       </c>
       <c r="G709" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="710" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A710" s="36" t="s">
         <v>840</v>
       </c>
@@ -28296,10 +28300,10 @@
         <v>8</v>
       </c>
       <c r="G710" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="711" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="711" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A711" s="36" t="s">
         <v>840</v>
       </c>
@@ -28319,10 +28323,10 @@
         <v>8</v>
       </c>
       <c r="G711" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="712" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A712" s="36" t="s">
         <v>840</v>
       </c>
@@ -28342,10 +28346,10 @@
         <v>8</v>
       </c>
       <c r="G712" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="713" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="713" spans="1:7" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A713" s="36" t="s">
         <v>840</v>
       </c>
@@ -28365,10 +28369,10 @@
         <v>8</v>
       </c>
       <c r="G713" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="714" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="714" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A714" s="36" t="s">
         <v>840</v>
       </c>
@@ -28388,10 +28392,10 @@
         <v>8</v>
       </c>
       <c r="G714" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="715" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A715" s="36" t="s">
         <v>840</v>
       </c>
@@ -28411,10 +28415,10 @@
         <v>8</v>
       </c>
       <c r="G715" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="716" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A716" s="36" t="s">
         <v>840</v>
       </c>
@@ -28434,10 +28438,10 @@
         <v>8</v>
       </c>
       <c r="G716" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="717" spans="1:7" s="14" customFormat="1" ht="42.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="717" spans="1:7" s="14" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A717" s="36" t="s">
         <v>840</v>
       </c>
@@ -28457,10 +28461,10 @@
         <v>8</v>
       </c>
       <c r="G717" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="718" spans="1:7" s="14" customFormat="1" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7" s="14" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A718" s="36" t="s">
         <v>840</v>
       </c>
@@ -28480,10 +28484,10 @@
         <v>8</v>
       </c>
       <c r="G718" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="719" spans="1:7" s="14" customFormat="1" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A719" s="36" t="s">
         <v>840</v>
       </c>
@@ -28503,10 +28507,10 @@
         <v>8</v>
       </c>
       <c r="G719" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="720" spans="1:7" s="14" customFormat="1" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7" s="14" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A720" s="36" t="s">
         <v>840</v>
       </c>
@@ -28526,10 +28530,10 @@
         <v>8</v>
       </c>
       <c r="G720" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="721" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A721" s="36" t="s">
         <v>840</v>
       </c>
@@ -28549,10 +28553,10 @@
         <v>8</v>
       </c>
       <c r="G721" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="722" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A722" s="36" t="s">
         <v>840</v>
       </c>
@@ -28572,10 +28576,10 @@
         <v>8</v>
       </c>
       <c r="G722" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="723" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A723" s="36" t="s">
         <v>840</v>
       </c>
@@ -28595,10 +28599,10 @@
         <v>8</v>
       </c>
       <c r="G723" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="724" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A724" s="36" t="s">
         <v>840</v>
       </c>
@@ -28618,10 +28622,10 @@
         <v>8</v>
       </c>
       <c r="G724" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="725" spans="1:7" s="14" customFormat="1" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7" s="14" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A725" s="36" t="s">
         <v>840</v>
       </c>
@@ -28641,10 +28645,10 @@
         <v>8</v>
       </c>
       <c r="G725" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="726" spans="1:7" s="14" customFormat="1" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726" spans="1:7" s="14" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A726" s="36" t="s">
         <v>840</v>
       </c>
@@ -28664,10 +28668,10 @@
         <v>8</v>
       </c>
       <c r="G726" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="727" spans="1:7" s="14" customFormat="1" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727" spans="1:7" s="14" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A727" s="36" t="s">
         <v>840</v>
       </c>
@@ -28685,10 +28689,10 @@
         <v>8</v>
       </c>
       <c r="G727" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="728" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A728" s="36" t="s">
         <v>840</v>
       </c>
@@ -28706,10 +28710,10 @@
         <v>8</v>
       </c>
       <c r="G728" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="729" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729" spans="1:7" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A729" s="36" t="s">
         <v>840</v>
       </c>
@@ -28727,10 +28731,10 @@
         <v>8</v>
       </c>
       <c r="G729" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="730" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="730" spans="1:7" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A730" s="36" t="s">
         <v>840</v>
       </c>
@@ -28750,10 +28754,10 @@
         <v>8</v>
       </c>
       <c r="G730" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="731" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="731" spans="1:7" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A731" s="36" t="s">
         <v>840</v>
       </c>
@@ -28773,10 +28777,10 @@
         <v>8</v>
       </c>
       <c r="G731" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="732" spans="1:7" s="14" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A732" s="36" t="s">
         <v>840</v>
       </c>
@@ -28796,10 +28800,10 @@
         <v>8</v>
       </c>
       <c r="G732" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="733" spans="1:7" s="14" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733" spans="1:7" s="14" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A733" s="41" t="s">
         <v>840</v>
       </c>
@@ -28819,10 +28823,10 @@
         <v>8</v>
       </c>
       <c r="G733" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="734" spans="1:7" s="14" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734" spans="1:7" s="14" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A734" s="41" t="s">
         <v>840</v>
       </c>
@@ -28842,10 +28846,10 @@
         <v>8</v>
       </c>
       <c r="G734" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="735" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735" spans="1:7" s="14" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A735" s="41" t="s">
         <v>840</v>
       </c>
@@ -28865,10 +28869,10 @@
         <v>8</v>
       </c>
       <c r="G735" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="736" spans="1:7" s="14" customFormat="1" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736" spans="1:7" s="14" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A736" s="41" t="s">
         <v>840</v>
       </c>
@@ -28888,10 +28892,10 @@
         <v>8</v>
       </c>
       <c r="G736" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="737" spans="1:7" s="14" customFormat="1" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="737" spans="1:7" s="14" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A737" s="41" t="s">
         <v>840</v>
       </c>
@@ -28911,10 +28915,10 @@
         <v>8</v>
       </c>
       <c r="G737" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="738" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A738" s="41" t="s">
         <v>840</v>
       </c>
@@ -28934,10 +28938,10 @@
         <v>8</v>
       </c>
       <c r="G738" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="739" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A739" s="41" t="s">
         <v>840</v>
       </c>
@@ -28957,10 +28961,10 @@
         <v>8</v>
       </c>
       <c r="G739" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="740" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A740" s="36" t="s">
         <v>840</v>
       </c>
@@ -28980,10 +28984,10 @@
         <v>8</v>
       </c>
       <c r="G740" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="741" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="741" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A741" s="36" t="s">
         <v>840</v>
       </c>
@@ -29003,10 +29007,10 @@
         <v>8</v>
       </c>
       <c r="G741" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="742" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A742" s="36" t="s">
         <v>840</v>
       </c>
@@ -29026,10 +29030,10 @@
         <v>8</v>
       </c>
       <c r="G742" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="743" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A743" s="36" t="s">
         <v>840</v>
       </c>
@@ -29049,10 +29053,10 @@
         <v>8</v>
       </c>
       <c r="G743" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="744" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A744" s="36" t="s">
         <v>840</v>
       </c>
@@ -29072,10 +29076,10 @@
         <v>8</v>
       </c>
       <c r="G744" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="745" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="745" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A745" s="36" t="s">
         <v>840</v>
       </c>
@@ -29095,10 +29099,10 @@
         <v>8</v>
       </c>
       <c r="G745" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="746" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="746" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A746" s="36" t="s">
         <v>840</v>
       </c>
@@ -29118,10 +29122,10 @@
         <v>8</v>
       </c>
       <c r="G746" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="747" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A747" s="36" t="s">
         <v>840</v>
       </c>
@@ -29141,10 +29145,10 @@
         <v>8</v>
       </c>
       <c r="G747" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="748" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A748" s="36" t="s">
         <v>840</v>
       </c>
@@ -29164,10 +29168,10 @@
         <v>8</v>
       </c>
       <c r="G748" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="749" spans="1:7" s="14" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="749" spans="1:7" s="14" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A749" s="36" t="s">
         <v>840</v>
       </c>
@@ -29187,10 +29191,10 @@
         <v>8</v>
       </c>
       <c r="G749" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="750" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="750" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A750" s="36" t="s">
         <v>840</v>
       </c>
@@ -29210,10 +29214,10 @@
         <v>8</v>
       </c>
       <c r="G750" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="751" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A751" s="36" t="s">
         <v>840</v>
       </c>
@@ -29233,10 +29237,10 @@
         <v>8</v>
       </c>
       <c r="G751" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="752" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="752" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A752" s="36" t="s">
         <v>840</v>
       </c>
@@ -29256,10 +29260,10 @@
         <v>8</v>
       </c>
       <c r="G752" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="753" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="753" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A753" s="36" t="s">
         <v>840</v>
       </c>
@@ -29279,10 +29283,10 @@
         <v>8</v>
       </c>
       <c r="G753" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="754" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="754" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A754" s="36" t="s">
         <v>840</v>
       </c>
@@ -29302,10 +29306,10 @@
         <v>8</v>
       </c>
       <c r="G754" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="755" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="755" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A755" s="36" t="s">
         <v>840</v>
       </c>
@@ -29325,10 +29329,10 @@
         <v>8</v>
       </c>
       <c r="G755" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="756" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A756" s="36" t="s">
         <v>840</v>
       </c>
@@ -29348,10 +29352,10 @@
         <v>8</v>
       </c>
       <c r="G756" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="757" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="757" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A757" s="36" t="s">
         <v>840</v>
       </c>
@@ -29371,10 +29375,10 @@
         <v>8</v>
       </c>
       <c r="G757" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="758" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A758" s="36" t="s">
         <v>840</v>
       </c>
@@ -29394,10 +29398,10 @@
         <v>8</v>
       </c>
       <c r="G758" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="759" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A759" s="36" t="s">
         <v>840</v>
       </c>
@@ -29417,10 +29421,10 @@
         <v>8</v>
       </c>
       <c r="G759" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="760" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A760" s="36" t="s">
         <v>840</v>
       </c>
@@ -29440,10 +29444,10 @@
         <v>8</v>
       </c>
       <c r="G760" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="761" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="761" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A761" s="36" t="s">
         <v>840</v>
       </c>
@@ -29463,10 +29467,10 @@
         <v>8</v>
       </c>
       <c r="G761" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="762" spans="1:7" s="14" customFormat="1" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" s="14" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A762" s="36" t="s">
         <v>840</v>
       </c>
@@ -29486,10 +29490,10 @@
         <v>8</v>
       </c>
       <c r="G762" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="763" spans="1:7" s="14" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A763" s="36" t="s">
         <v>925</v>
       </c>
@@ -29507,10 +29511,10 @@
         <v>8</v>
       </c>
       <c r="G763" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="764" spans="1:7" s="14" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A764" s="36" t="s">
         <v>925</v>
       </c>
@@ -29528,7 +29532,7 @@
         <v>8</v>
       </c>
       <c r="G764" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="765" spans="1:7" s="14" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30872,22 +30876,22 @@
       </c>
     </row>
     <row r="827" spans="1:7" s="29" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A827" s="37" t="s">
+      <c r="A827" s="42" t="s">
         <v>989</v>
       </c>
-      <c r="B827" s="24" t="s">
+      <c r="B827" s="44" t="s">
         <v>990</v>
       </c>
-      <c r="C827" s="27" t="s">
+      <c r="C827" s="43" t="s">
         <v>1955</v>
       </c>
-      <c r="D827" s="26" t="s">
+      <c r="D827" s="43" t="s">
         <v>991</v>
       </c>
-      <c r="E827" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F827" s="28">
+      <c r="E827" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F827" s="45">
         <v>8</v>
       </c>
       <c r="G827" s="29">
@@ -30987,22 +30991,22 @@
       </c>
     </row>
     <row r="832" spans="1:7" s="29" customFormat="1" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A832" s="37" t="s">
+      <c r="A832" s="42" t="s">
         <v>989</v>
       </c>
-      <c r="B832" s="24" t="s">
+      <c r="B832" s="44" t="s">
         <v>996</v>
       </c>
-      <c r="C832" s="27" t="s">
+      <c r="C832" s="43" t="s">
         <v>1960</v>
       </c>
-      <c r="D832" s="26" t="s">
+      <c r="D832" s="43" t="s">
         <v>2768</v>
       </c>
-      <c r="E832" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F832" s="28">
+      <c r="E832" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F832" s="45">
         <v>8</v>
       </c>
       <c r="G832" s="29">

</xml_diff>